<commit_message>
Add tests for AllItems and About button
</commit_message>
<xml_diff>
--- a/src/test/java/SwagLabs/TestData.xlsx
+++ b/src/test/java/SwagLabs/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5790" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5796"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Valid Username</t>
   </si>
@@ -60,9 +60,6 @@
     <t>performance_glitch_user</t>
   </si>
   <si>
-    <t>Profile page</t>
-  </si>
-  <si>
     <t>https://www.saucedemo.com/inventory.html</t>
   </si>
   <si>
@@ -73,6 +70,15 @@
   </si>
   <si>
     <t>123secret_sauce</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>About page</t>
+  </si>
+  <si>
+    <t>https://saucelabs.com/</t>
   </si>
 </sst>
 </file>
@@ -403,34 +409,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
   </sheetData>
@@ -445,20 +456,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -483,23 +494,23 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add class "SwagLabsItemsPage" Add class "SwagLabsItemsPageTest"
</commit_message>
<xml_diff>
--- a/src/test/java/SwagLabs/TestData.xlsx
+++ b/src/test/java/SwagLabs/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Valid Username</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>https://saucelabs.com/</t>
+  </si>
+  <si>
+    <t>Items URL</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=4</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=0</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=1</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=5</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=2</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory-item.html?id=3</t>
   </si>
 </sst>
 </file>
@@ -407,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +439,7 @@
     <col min="1" max="1" width="33.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -431,6 +452,9 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -442,13 +466,42 @@
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>